<commit_message>
Create Sheet#max_column Sheet#max_row and related rspec
</commit_message>
<xml_diff>
--- a/spec/xlsx_files/xlsx_test1.xlsx
+++ b/spec/xlsx_files/xlsx_test1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\ruby\xlsx-DSL\spec\xlsx_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{926656C1-3533-47B6-9DE8-AE458F848FFA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D247F52F-5536-48AE-B110-242123D72DCA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet10" sheetId="10" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>D7</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -40,6 +40,14 @@
   </si>
   <si>
     <t>E68cyan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F27</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -391,8 +399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C5F4A0C-FF31-42DA-8DFF-550BD31FC0D0}">
   <dimension ref="B3:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -422,10 +430,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C45BD08-E68A-4D5F-99AF-CEEC9CF28BDF}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -433,14 +449,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3034BB4-399F-4ED6-AEEA-02DACA93CBA8}">
-  <dimension ref="A1"/>
+  <dimension ref="F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="27" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Refator Sheet#[] which calls private methods which are retrieve_rows & retrieve_columns
</commit_message>
<xml_diff>
--- a/spec/xlsx_files/xlsx_test1.xlsx
+++ b/spec/xlsx_files/xlsx_test1.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\ruby\xlsx-DSL\spec\xlsx_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B430262-AB53-4951-AB22-13E320CE3B29}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89202271-F190-44F3-8F4B-08460D6B362C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet10" sheetId="10" r:id="rId1"/>
     <sheet name="some" sheetId="11" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="13" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="14" r:id="rId4"/>
-    <sheet name="cell" sheetId="15" r:id="rId5"/>
-    <sheet name="last" sheetId="12" r:id="rId6"/>
+    <sheet name="range" sheetId="17" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="14" r:id="rId5"/>
+    <sheet name="cell" sheetId="15" r:id="rId6"/>
+    <sheet name="last" sheetId="12" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -404,8 +405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C5F4A0C-FF31-42DA-8DFF-550BD31FC0D0}">
   <dimension ref="B1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -478,6 +479,78 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D8ECDE3-3C3B-495E-9254-5F60EEBBB104}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1">
+        <v>3</v>
+      </c>
+      <c r="D1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>14</v>
+      </c>
+      <c r="C4">
+        <v>15</v>
+      </c>
+      <c r="D4">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3034BB4-399F-4ED6-AEEA-02DACA93CBA8}">
   <dimension ref="F27"/>
   <sheetViews>
@@ -498,7 +571,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E415BE4-A107-4BEC-AE8C-2C656DD5BD8F}">
   <dimension ref="A1:K74"/>
   <sheetViews>
@@ -573,7 +646,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AA2DCBA-D571-4053-9351-F6C9819B1E80}">
   <dimension ref="E68"/>
   <sheetViews>

</xml_diff>